<commit_message>
- 更新 luban 修复一些bug - 修复 MiniDesignerConfigsTemplate和Benchmark配置无法生成的bug
</commit_message>
<xml_diff>
--- a/Benchmark/Datas/tables.xlsx
+++ b/Benchmark/Datas/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\Benchmark\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDAC719-2E77-40E3-85E2-5AC422CDCCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F922BF-5F17-4063-BE83-9651633714F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30000" yWindow="2145" windowWidth="25335" windowHeight="12915" xr2:uid="{947BE16E-96E8-4B86-802B-E77C4FDA60B0}"/>
+    <workbookView xWindow="-1005" yWindow="2415" windowWidth="25335" windowHeight="12915" xr2:uid="{947BE16E-96E8-4B86-802B-E77C4FDA60B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="530">
   <si>
     <t>##</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1641,6 +1641,10 @@
   </si>
   <si>
     <t>patch_input</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>output</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2025,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9106277-D8F0-4267-8ADA-C7EA4498DD01}">
-  <dimension ref="A1:K504"/>
+  <dimension ref="A1:L504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2041,12 +2045,12 @@
     <col min="10" max="10" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -2077,8 +2081,11 @@
       <c r="K2" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2107,7 +2114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
@@ -2127,7 +2134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -2141,7 +2148,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>26</v>
       </c>
@@ -2155,7 +2162,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>27</v>
       </c>
@@ -2169,7 +2176,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -2183,7 +2190,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>29</v>
       </c>
@@ -2197,7 +2204,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>30</v>
       </c>
@@ -2211,7 +2218,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -2225,7 +2232,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -2239,7 +2246,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>33</v>
       </c>
@@ -2253,7 +2260,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -2267,7 +2274,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>35</v>
       </c>
@@ -2281,7 +2288,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>36</v>
       </c>

</xml_diff>